<commit_message>
Added garbo data and updated the rest for consistency
</commit_message>
<xml_diff>
--- a/database/test-import-data/data.xlsx
+++ b/database/test-import-data/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saahi\OneDrive\Desktop\FTSP\week 5\project files\csv to sql\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saahi\OneDrive\Desktop\overseas-travel-database-management-system\database\test-import-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A361132-BDC3-489B-8C3F-7648EB981E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F76DAEA5-95DA-45EE-8B03-7240E5A2208D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{06BB8B05-F846-4CCD-AA37-3D2CA17146F6}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>adminNo</t>
   </si>
@@ -52,29 +52,65 @@
     <t>gender</t>
   </si>
   <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>Green</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>gaul</t>
-  </si>
-  <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>citizenshipStatus</t>
+  </si>
+  <si>
+    <t>course</t>
+  </si>
+  <si>
+    <t>stage</t>
+  </si>
+  <si>
+    <t>pemGroup</t>
+  </si>
+  <si>
+    <t>212345A</t>
+  </si>
+  <si>
+    <t>XLSX Uno</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Singapore citizen</t>
+  </si>
+  <si>
+    <t>C02</t>
+  </si>
+  <si>
+    <t>MI2002</t>
+  </si>
+  <si>
+    <t>212346A</t>
+  </si>
+  <si>
+    <t>212347A</t>
+  </si>
+  <si>
+    <t>XLSX Dos</t>
+  </si>
+  <si>
+    <t>XLSX Tres</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -443,48 +479,112 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CB91F20-FB48-493B-927B-380DE584D14D}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="7" max="7" width="13.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>3</v>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>4</v>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>